<commit_message>
change individual_jtg and group_jtg excel
</commit_message>
<xml_diff>
--- a/public/group_jtg.xlsx
+++ b/public/group_jtg.xlsx
@@ -529,15 +529,108 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>175260</xdr:colOff>
+      <xdr:colOff>320041</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>200329</xdr:rowOff>
+      <xdr:rowOff>248504</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>716280</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>746759</xdr:rowOff>
+      <xdr:rowOff>787237</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="図 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3337561" y="9141044"/>
+          <a:ext cx="533399" cy="538733"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>683400</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>96602</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>586798</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>784860</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="図 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4440060" y="8989142"/>
+          <a:ext cx="688258" cy="688258"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>319542</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>594359</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>858275</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -560,8 +653,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3192780" y="9092869"/>
-          <a:ext cx="541020" cy="546430"/>
+          <a:off x="3771900" y="18097002"/>
+          <a:ext cx="533399" cy="538733"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -572,16 +665,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>264300</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>124740</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1430159</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>30480</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>12840</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2118417</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>863518</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -604,101 +697,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4805820" y="9017280"/>
-          <a:ext cx="680580" cy="680580"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>319505</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>858239</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="図 5"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3787140" y="18096965"/>
-          <a:ext cx="533400" cy="538734"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1567320</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>2247900</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>871080</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="図 6"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5278260" y="17967960"/>
-          <a:ext cx="680580" cy="680580"/>
+          <a:off x="5141099" y="17952720"/>
+          <a:ext cx="688258" cy="688258"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1000,7 +1000,7 @@
   <dimension ref="A1:G986"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.3984375" defaultRowHeight="15" customHeight="1"/>
@@ -8030,8 +8030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1025"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H51" sqref="H51"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H53" sqref="H53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.3984375" defaultRowHeight="15" customHeight="1"/>
@@ -14587,8 +14587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1003"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.3984375" defaultRowHeight="15" customHeight="1"/>

</xml_diff>